<commit_message>
sua lai lay file excel
</commit_message>
<xml_diff>
--- a/phieunhap.xlsx
+++ b/phieunhap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Do AN\Nhom-7-QL-Kho-Hang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A767D2-8D89-423D-B2F2-D08ACB7E68E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0A6F76-1125-49B1-873D-9FA00703FFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>TRƯỜNG ĐẠI HỌC CÔNG THƯƠNG TP.HCM</t>
   </si>
@@ -96,21 +96,6 @@
     <t>Huawei P40</t>
   </si>
   <si>
-    <t>Tổng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.000,00 </t>
-  </si>
-  <si>
-    <t>VNĐ</t>
-  </si>
-  <si>
-    <t>Tổng tiền (bằng chữ):</t>
-  </si>
-  <si>
-    <t>Chứng từ kèm theo</t>
-  </si>
-  <si>
     <t>TP.HCM, Ngày ….. Tháng ….. Năm …..</t>
   </si>
   <si>
@@ -124,6 +109,18 @@
   </si>
   <si>
     <t>Trần Thị Lan</t>
+  </si>
+  <si>
+    <t>SP09</t>
+  </si>
+  <si>
+    <t>SP03</t>
+  </si>
+  <si>
+    <t>Xiaomi Mi 11</t>
+  </si>
+  <si>
+    <t>OnePlus 9</t>
   </si>
 </sst>
 </file>
@@ -173,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -222,53 +219,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,27 +235,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -578,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -973,58 +942,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1049,156 +1018,197 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+      <c r="A14" s="3">
         <v>1</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="3">
         <v>30</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="3">
         <v>22000</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="3">
         <v>660000</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="5">
         <v>2</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="3">
         <v>10</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="3">
         <v>15000</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="3">
         <v>150000</v>
       </c>
-      <c r="G15" s="11"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="3">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18000</v>
+      </c>
+      <c r="F16" s="3">
+        <v>660000</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="18">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="3">
+        <v>20</v>
+      </c>
+      <c r="E17" s="3">
+        <v>28000</v>
+      </c>
+      <c r="F17" s="3">
+        <v>150000</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="B24" s="8"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E27" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="4"/>
+      <c r="F29" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E8:G8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E23:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>